<commit_message>
Basic gesture classification. Everything is either a horizontal r->l line or l->r line. Oh well.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="282" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="423" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -135,7 +135,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -168,7 +168,7 @@
         <v>0.999988425925926</v>
       </c>
       <c r="D3" s="0" t="n">
-        <f aca="false"> ROUND(ABS(C3-B3) * 24)</f>
+        <f aca="false">ROUND(ABS(C3-B3) * 24, 1)</f>
         <v>2</v>
       </c>
     </row>
@@ -183,7 +183,7 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="D4" s="0" t="n">
-        <f aca="false"> ABS(C4-B4) * 24</f>
+        <f aca="false">ROUND(ABS(C4-B4) * 24, 1)</f>
         <v>2</v>
       </c>
     </row>
@@ -198,7 +198,7 @@
         <v>0.145833333333333</v>
       </c>
       <c r="D5" s="0" t="n">
-        <f aca="false"> ABS(C5-B5) * 24</f>
+        <f aca="false">ROUND(ABS(C5-B5) * 24, 1)</f>
         <v>2</v>
       </c>
     </row>
@@ -213,55 +213,73 @@
         <v>0.6875</v>
       </c>
       <c r="D6" s="0" t="n">
-        <f aca="false"> ABS(C6-B6) * 24</f>
+        <f aca="false">ROUND(ABS(C6-B6) * 24, 1)</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>41958</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.979166666666667</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0.999988425925926</v>
+      </c>
       <c r="D7" s="0" t="n">
-        <f aca="false"> ABS(C7-B7) * 24</f>
-        <v>0</v>
+        <f aca="false">ROUND(ABS(C7-B7) * 24, 1)</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>41959</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D8" s="0" t="n">
-        <f aca="false"> ABS(C8-B8) * 24</f>
-        <v>0</v>
+        <f aca="false">ROUND(ABS(C8-B8) * 24, 1)</f>
+        <v>4.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="0" t="n">
-        <f aca="false"> ABS(C9-B9) * 24</f>
+        <f aca="false">ROUND(ABS(C9-B9) * 24, 1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D10" s="0" t="n">
-        <f aca="false"> ABS(C10-B10) * 24</f>
+        <f aca="false">ROUND(ABS(C10-B10) * 24, 1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D11" s="0" t="n">
-        <f aca="false"> ABS(C11-B11) * 24</f>
+        <f aca="false">ROUND(ABS(C11-B11) * 24, 1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="n">
-        <f aca="false"> ABS(C12-B12) * 24</f>
+        <f aca="false">ROUND(ABS(C12-B12) * 24, 1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="0" t="n">
-        <f aca="false"> ABS(C13-B13) * 24</f>
+        <f aca="false">ROUND(ABS(C13-B13) * 24, 1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="0" t="n">
-        <f aca="false"> ABS(C14-B14) * 24</f>
+        <f aca="false">ROUND(ABS(C14-B14) * 24, 1)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved items around, removed unnecessary items from directory
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -132,10 +132,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -248,21 +248,48 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>41959</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0.999988425925926</v>
+      </c>
       <c r="D9" s="0" t="n">
         <f aca="false">ROUND(ABS(C9-B9) * 24, 1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>41960</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0.0833333333333333</v>
+      </c>
       <c r="D10" s="0" t="n">
         <f aca="false">ROUND(ABS(C10-B10) * 24, 1)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>41961</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>0.145833333333333</v>
+      </c>
       <c r="D11" s="0" t="n">
         <f aca="false">ROUND(ABS(C11-B11) * 24, 1)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,6 +308,12 @@
       <c r="D14" s="0" t="n">
         <f aca="false">ROUND(ABS(C14-B14) * 24, 1)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="0" t="n">
+        <f aca="false"> SUM(D3:D25)</f>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new version of file, restructured slightly to provide easy to use API format. Added example code to allow user to display everything in a Tkinter window. It works nicely.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -43,6 +43,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -135,7 +136,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -293,27 +294,99 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>41964</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>0.708333333333333</v>
+      </c>
       <c r="D12" s="0" t="n">
         <f aca="false">ROUND(ABS(C12-B12) * 24, 1)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>41964</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>0.958333333333333</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>0.999988425925926</v>
+      </c>
       <c r="D13" s="0" t="n">
         <f aca="false">ROUND(ABS(C13-B13) * 24, 1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>41965</v>
+      </c>
+      <c r="B14" s="2" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="2" t="n">
+        <v>0.0833333333333333</v>
+      </c>
       <c r="D14" s="0" t="n">
         <f aca="false">ROUND(ABS(C14-B14) * 24, 1)</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>41965</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">ROUND(ABS(C15-B15) * 24, 1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>41966</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">ROUND(ABS(C16-B16) * 24, 1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>41966</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">ROUND(ABS(C17-B17) * 24, 1)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="0" t="n">
-        <f aca="false"> SUM(D3:D25)</f>
-        <v>21</v>
+        <f aca="false">SUM(D3:D25)</f>
+        <v>39.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified readme, added updates file.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -43,7 +43,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,7 +135,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -383,10 +382,40 @@
         <v>4</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>41968</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">ROUND(ABS(C18-B18) * 24, 1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>41969</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">ROUND(ABS(C19-B19) * 24, 1)</f>
+        <v>5</v>
+      </c>
+    </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="0" t="n">
         <f aca="false">SUM(D3:D25)</f>
-        <v>39.5</v>
+        <v>46.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spent a bunch of time again on trying to implement circle detection for the palm. Many appropriate circles are being generated, I don't know how to choose between them.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -43,6 +43,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -135,7 +136,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -412,10 +413,40 @@
         <v>5</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>41972</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0.791666666666667</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">ROUND(ABS(C20-B20) * 24, 1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>41973</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">ROUND(ABS(C21-B21) * 24, 1)</f>
+        <v>4.5</v>
+      </c>
+    </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="0" t="n">
         <f aca="false">SUM(D3:D25)</f>
-        <v>46.5</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up code and restructured it. Removed many unnecessary fragments of code. Everything old has been deleted, I'll probably end up making a new directory with unnecessary fragments instead.
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -136,7 +136,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -458,10 +458,25 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>41975</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">ROUND(ABS(C23-B23) * 24, 1)</f>
+        <v>3.5</v>
+      </c>
+    </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D26" s="0" t="n">
         <f aca="false">SUM(D3:D25)</f>
-        <v>59.5</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>